<commit_message>
Refactoring vendor bots for new parsing
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/OrderFiles/Copper Horse Coffee/combined_orders.xlsx
+++ b/WorkBot/main/backend/ordering/OrderFiles/Copper Horse Coffee/combined_orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Andrew\Projects\RandomStuff\WorkBot\main\backend\ordering\OrderFiles\Copper Horse Coffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B7768-670E-41DE-82DD-622CD8648F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02328060-91E1-4E14-A68E-F7CCA5615E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,39 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Item</t>
   </si>
   <si>
+    <t>Easthill</t>
+  </si>
+  <si>
+    <t>Bakery</t>
+  </si>
+  <si>
+    <t>Downtown</t>
+  </si>
+  <si>
+    <t>Triphammer</t>
+  </si>
+  <si>
     <t>Collegetown</t>
   </si>
   <si>
-    <t>Downtown</t>
-  </si>
-  <si>
-    <t>Bakery</t>
-  </si>
-  <si>
-    <t>Triphammer</t>
-  </si>
-  <si>
     <t>Copper Horse - Warhorse 5lb</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Copper Horse - Warhorse Blend (12oz)</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Copper Horse - Warhorse Blend (12oz)</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Copper Horse - Rumble Pony (12oz)</t>
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>Copper Horse - Rumble Pony (12oz)</t>
   </si>
   <si>
     <t>Copper Horse - Clocktower Espresso (12oz)</t>
@@ -94,16 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,98 +422,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>